<commit_message>
Change indexeres method to LINQ. Temporary storage, KnxObject and KnxScene will have big changes.
</commit_message>
<xml_diff>
--- a/BedivereKnx.GUI/data.xlsx
+++ b/BedivereKnx.GUI/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program\Ouroboros\BedivereKnx\BedivereKnx.GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB7FDC6-09D2-402A-A5E9-0D28D7449019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC9958D-C2D1-4CF8-B7C0-7E6A99EA586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7896,7 +7896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9671D8-C670-4FF9-9F5F-C699E4CE0AC7}">
   <dimension ref="A1:K446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -7904,7 +7904,7 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" style="3" customWidth="1"/>
     <col min="5" max="5" width="30.5546875" style="3" bestFit="1" customWidth="1"/>

</xml_diff>